<commit_message>
vault backup: 2023-03-27 14:33:29
</commit_message>
<xml_diff>
--- a/Research/情感语音/{2}_论文记录/情感识别论文统计.xlsx
+++ b/Research/情感语音/{2}_论文记录/情感识别论文统计.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\{3}_进修\{4}_笔记\Research\情感语音\{2}_论文记录\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4178431A-BBBF-4781-8649-70D7D7AAB16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F32E70-01C9-4139-A4C4-F8D8D52FF60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5448" yWindow="8820" windowWidth="15276" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="G3" sqref="G3:G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1228,7 @@
         <v>100.21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>0.77029999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>149</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>92</v>
       </c>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>199</v>
       </c>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="H95" s="6"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>60</v>
       </c>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="H96" s="6"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>197</v>
       </c>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>200</v>
       </c>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>172</v>
       </c>
@@ -3265,16 +3265,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G107" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
     <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="语音"/>
+      <filters>
         <filter val="语音+视频"/>
-        <filter val="语音-视频"/>
+        <filter val="语音-视频-文本"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G107">

</xml_diff>

<commit_message>
vault backup: 2023-04-29 18:47:28
</commit_message>
<xml_diff>
--- a/Research/情感语音/{2}_论文记录/情感识别论文统计.xlsx
+++ b/Research/情感语音/{2}_论文记录/情感识别论文统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\{3}_进修\{4}_笔记\Research\情感语音\{2}_论文记录\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F32E70-01C9-4139-A4C4-F8D8D52FF60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA5A4E-4A4B-42C3-B649-5534C16FB209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1104" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,391 +410,392 @@
     <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks</t>
   </si>
   <si>
+    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions</t>
+  </si>
+  <si>
+    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Meta-Learning for Low-Resource Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition</t>
+  </si>
+  <si>
+    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks</t>
+  </si>
+  <si>
+    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection</t>
+  </si>
+  <si>
+    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions</t>
+  </si>
+  <si>
+    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
+  </si>
+  <si>
+    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
+  </si>
+  <si>
+    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
+  </si>
+  <si>
+    <t>Temporal Context in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
+  </si>
+  <si>
+    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
+  </si>
+  <si>
+    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
+  </si>
+  <si>
+    <t>Emotion Carrier Recognition from Personal Narratives</t>
+  </si>
+  <si>
+    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
+  </si>
+  <si>
+    <t>Emotional Prosody Control for Speech Generation</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
+  </si>
+  <si>
+    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
+  </si>
+  <si>
+    <t>Speaker Attentive Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
+  </si>
+  <si>
+    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
+  </si>
+  <si>
+    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
+  </si>
+  <si>
+    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
+  </si>
+  <si>
+    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
+  </si>
+  <si>
+    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
+  </si>
+  <si>
+    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMU-MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音+视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+ESD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmoDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.5±1.0%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wF1 78.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSI+CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音-视频-文本 </t>
+  </si>
+  <si>
+    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本 </t>
+  </si>
+  <si>
+    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wf1 65.85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MELD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emo-DB+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.6± 4.7% - 61.7±9.2%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMUMOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+NNIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-IMPROV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.613 ± 0.018%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+Att-HACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS+Emo-DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音 </t>
+  </si>
+  <si>
+    <t>67.2 ± 0.7%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95.90 ± 4.31%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本   </t>
+  </si>
+  <si>
+    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition with Multi-Task Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Multimodal Emotion Recognition with Capsule Graph Convolutional Based Representation Fusion</t>
-  </si>
-  <si>
-    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions</t>
-  </si>
-  <si>
-    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Meta-Learning for Low-Resource Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition</t>
-  </si>
-  <si>
-    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks</t>
-  </si>
-  <si>
-    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection</t>
-  </si>
-  <si>
-    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions</t>
-  </si>
-  <si>
-    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
-  </si>
-  <si>
-    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
-  </si>
-  <si>
-    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
-  </si>
-  <si>
-    <t>Temporal Context in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
-  </si>
-  <si>
-    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
-  </si>
-  <si>
-    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
-  </si>
-  <si>
-    <t>Emotion Carrier Recognition from Personal Narratives</t>
-  </si>
-  <si>
-    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
-  </si>
-  <si>
-    <t>Emotional Prosody Control for Speech Generation</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
-  </si>
-  <si>
-    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
-  </si>
-  <si>
-    <t>Speaker Attentive Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
-  </si>
-  <si>
-    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
-  </si>
-  <si>
-    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
-  </si>
-  <si>
-    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
-  </si>
-  <si>
-    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
-  </si>
-  <si>
-    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
-  </si>
-  <si>
-    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMU-MOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音+视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+ESD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EmoDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>87.5±1.0%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wF1 78.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSI+CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音-视频-文本 </t>
-  </si>
-  <si>
-    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本 </t>
-  </si>
-  <si>
-    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wf1 65.85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emo-DB+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.6± 4.7% - 61.7±9.2%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMUMOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+NNIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-IMPROV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.613 ± 0.018%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+Att-HACK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS+Emo-DB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音 </t>
-  </si>
-  <si>
-    <t>67.2 ± 0.7%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95.90 ± 4.31%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本   </t>
-  </si>
-  <si>
-    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition with Multi-Task Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>√</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -893,6 +894,1097 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="52"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0190280795615676E-16"/>
+                  <c:y val="-3.8514770114201798E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="9.1560840071068725E-2"/>
+                      <c:h val="6.7328490706082947E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-E383-44AB-BB35-0A09C2A8E9B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$113:$A$166</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>0.57599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58189999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60429999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6169</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62680000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65849999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.66900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.67420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.67900000000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68169999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68189999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.68210000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.6976</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.70109999999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.70399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7046</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.70540000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.70820000000000005</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.7248</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.72829999999999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.73040000000000005</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.73219999999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.73499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.75209999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.75600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.75929999999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.76100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.76100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.76170000000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.7631</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.76500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.77029999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.77100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.77359999999999995</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.77759999999999996</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.78149999999999997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.78500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.79520000000000002</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.79530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.80030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.83189999999999997</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.84450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.84499999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E383-44AB-BB35-0A09C2A8E9B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="732520920"/>
+        <c:axId val="732522232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="732520920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="732522232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="732522232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="732520920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129989</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>62754</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1645024</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>116542</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7636FA37-35F7-41D5-BDD9-4558124AC131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1159,10 +2251,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G72"/>
+    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G136" sqref="G136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1204,9 +2296,9 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>55</v>
@@ -1254,7 +2346,7 @@
         <v>84.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -1323,12 +2415,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>54</v>
@@ -1346,17 +2438,17 @@
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G8" s="1"/>
       <c r="L8" s="1">
         <v>79.53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -1377,15 +2469,15 @@
         <v>79.52</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G10" s="6">
         <v>0.65600000000000003</v>
@@ -1396,10 +2488,10 @@
     </row>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G11" s="1"/>
       <c r="J11" s="10">
@@ -1409,7 +2501,7 @@
         <v>78.150000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1434,7 +2526,7 @@
     </row>
     <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>55</v>
@@ -1493,12 +2585,12 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>54</v>
@@ -1516,13 +2608,13 @@
     </row>
     <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>59</v>
@@ -1534,7 +2626,7 @@
         <v>76.17</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -1557,10 +2649,10 @@
     </row>
     <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="3"/>
@@ -1568,15 +2660,15 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G20" s="6">
         <v>0.6169</v>
@@ -1591,7 +2683,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>55</v>
@@ -1600,10 +2692,10 @@
         <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G21" s="2">
         <v>73.22</v>
@@ -1662,7 +2754,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -1687,17 +2779,17 @@
     </row>
     <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G25" s="1"/>
       <c r="L25" s="1">
         <v>73.040000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -1722,10 +2814,10 @@
     </row>
     <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G27" s="1"/>
       <c r="J27" s="10">
@@ -1737,10 +2829,10 @@
     </row>
     <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G28" s="1"/>
       <c r="J28" s="10">
@@ -1776,19 +2868,19 @@
     </row>
     <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H30" s="3"/>
       <c r="J30" s="10">
@@ -1798,7 +2890,7 @@
         <v>70.459999999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
@@ -1824,7 +2916,7 @@
     </row>
     <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>55</v>
@@ -1835,15 +2927,15 @@
         <v>70.11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1881,7 +2973,7 @@
     </row>
     <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>14</v>
@@ -1902,27 +2994,27 @@
     </row>
     <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L36" s="1">
         <v>68.17</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>55</v>
@@ -1966,7 +3058,7 @@
     </row>
     <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>14</v>
@@ -2001,9 +3093,9 @@
         <v>65.599999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>56</v>
@@ -2027,10 +3119,10 @@
     </row>
     <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="3"/>
@@ -2041,15 +3133,15 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>53</v>
@@ -2065,7 +3157,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>88</v>
       </c>
@@ -2088,21 +3180,21 @@
         <v>61.69</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J45" s="10">
         <v>73.040000000000006</v>
@@ -2113,10 +3205,10 @@
     </row>
     <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G46" s="1"/>
       <c r="J46" s="10">
@@ -2126,15 +3218,15 @@
         <v>60.43</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -2151,10 +3243,10 @@
     </row>
     <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G48" s="1"/>
       <c r="J48" s="10">
@@ -2164,7 +3256,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>87</v>
       </c>
@@ -2188,9 +3280,9 @@
         <v>36.58</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>55</v>
@@ -2212,18 +3304,18 @@
         <v>0.77029999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2236,13 +3328,13 @@
     </row>
     <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>53</v>
@@ -2255,7 +3347,7 @@
     </row>
     <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>55</v>
@@ -2271,10 +3363,10 @@
     </row>
     <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2285,15 +3377,15 @@
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>59</v>
@@ -2309,7 +3401,7 @@
         <v>0.62680000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -2333,9 +3425,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>55</v>
@@ -2344,7 +3436,7 @@
         <v>54</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G57" s="6">
         <v>0.84450000000000003</v>
@@ -2357,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -2381,15 +3473,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>59</v>
@@ -2405,12 +3497,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>54</v>
@@ -2450,9 +3542,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>55</v>
@@ -2476,7 +3568,7 @@
     </row>
     <row r="63" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>55</v>
@@ -2494,23 +3586,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H64" s="8"/>
       <c r="J64" s="11">
@@ -2520,15 +3612,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -2544,9 +3636,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>14</v>
@@ -2568,9 +3660,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>55</v>
@@ -2579,7 +3671,7 @@
         <v>54</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G67" s="8">
         <v>0.73040000000000005</v>
@@ -2594,7 +3686,7 @@
     </row>
     <row r="68" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>14</v>
@@ -2614,12 +3706,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>54</v>
@@ -2636,15 +3728,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H70" s="8"/>
       <c r="J70" s="11"/>
@@ -2673,9 +3765,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>14</v>
@@ -2712,9 +3804,9 @@
       <c r="H73" s="8"/>
       <c r="J73" s="11"/>
     </row>
-    <row r="74" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>55</v>
@@ -2728,7 +3820,7 @@
       <c r="H74" s="8"/>
       <c r="J74" s="11"/>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -2746,7 +3838,7 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
@@ -2784,9 +3876,9 @@
       </c>
       <c r="J77" s="11"/>
     </row>
-    <row r="78" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>56</v>
@@ -2795,22 +3887,22 @@
         <v>54</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J78" s="11"/>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
@@ -2820,18 +3912,18 @@
       </c>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G80" s="6">
         <v>0.77100000000000002</v>
@@ -2840,29 +3932,29 @@
     </row>
     <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H81" s="1"/>
     </row>
     <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>14</v>
@@ -2878,7 +3970,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>62</v>
       </c>
@@ -2896,18 +3988,18 @@
       </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -2918,10 +4010,10 @@
     </row>
     <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -2944,40 +4036,40 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G88" s="6">
         <v>0.76100000000000001</v>
       </c>
       <c r="H88" s="6"/>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -2997,7 +4089,7 @@
     </row>
     <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>55</v>
@@ -3007,18 +4099,18 @@
     </row>
     <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -3036,37 +4128,37 @@
       </c>
       <c r="H93" s="6"/>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G94" s="6">
         <v>0.70399999999999996</v>
       </c>
       <c r="H94" s="6"/>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G95" s="6">
         <v>0.61399999999999999</v>
       </c>
       <c r="H95" s="6"/>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>60</v>
       </c>
@@ -3087,18 +4179,18 @@
       </c>
       <c r="H96" s="6"/>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G97" s="6">
         <v>0.78149999999999997</v>
@@ -3107,30 +4199,30 @@
     </row>
     <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="6"/>
     </row>
     <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
     <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>55</v>
@@ -3138,60 +4230,60 @@
       <c r="G100" s="1"/>
       <c r="H100" s="6"/>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G101" s="6">
         <v>0.75</v>
       </c>
       <c r="H101" s="6"/>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G102" s="6">
         <v>0.66900000000000004</v>
       </c>
       <c r="H102" s="6"/>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G103" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>55</v>
@@ -3207,12 +4299,12 @@
       </c>
       <c r="H104" s="6"/>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>54</v>
@@ -3224,7 +4316,7 @@
     </row>
     <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>8</v>
@@ -3233,7 +4325,7 @@
         <v>32</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>16</v>
@@ -3243,18 +4335,18 @@
       </c>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -3263,20 +4355,342 @@
       </c>
       <c r="H107" s="6"/>
     </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>0.36580000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="B113" s="10"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>0.58189999999999997</v>
+      </c>
+      <c r="B114" s="10"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <v>0.60429999999999995</v>
+      </c>
+      <c r="B115" s="10"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="6">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="B116" s="10"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="6">
+        <v>0.6169</v>
+      </c>
+      <c r="B117" s="10"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
+        <v>0.62680000000000002</v>
+      </c>
+      <c r="B118" s="10"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="8">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="B119" s="10"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="B120" s="10"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="8">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="B121" s="10"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="6">
+        <v>0.65529999999999999</v>
+      </c>
+      <c r="B122" s="10"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="6">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="B123" s="10"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="6">
+        <v>0.65849999999999997</v>
+      </c>
+      <c r="B124" s="10"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="3">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="B125" s="10"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="6">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="B126" s="10"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="8">
+        <v>0.67420000000000002</v>
+      </c>
+      <c r="B127" s="10"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="6">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="B128" s="10"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="8">
+        <v>0.68169999999999997</v>
+      </c>
+      <c r="B129" s="10"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="3">
+        <v>0.68189999999999995</v>
+      </c>
+      <c r="B130" s="10"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="3">
+        <v>0.68210000000000004</v>
+      </c>
+      <c r="B131" s="10"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="8">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="B132" s="10"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="3">
+        <v>0.6976</v>
+      </c>
+      <c r="B133" s="10"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="8">
+        <v>0.70109999999999995</v>
+      </c>
+      <c r="B134" s="10"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="6">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="B135" s="10"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="3">
+        <v>0.7046</v>
+      </c>
+      <c r="B136" s="10"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="3">
+        <v>0.70540000000000003</v>
+      </c>
+      <c r="B137" s="10"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="6">
+        <v>0.70820000000000005</v>
+      </c>
+      <c r="B138" s="10"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="8">
+        <v>0.7248</v>
+      </c>
+      <c r="B139" s="10"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="6">
+        <v>0.72829999999999995</v>
+      </c>
+      <c r="B140" s="10"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="8">
+        <v>0.73040000000000005</v>
+      </c>
+      <c r="B141" s="10"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="3">
+        <v>0.73219999999999996</v>
+      </c>
+      <c r="B142" s="10"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="6">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="B143" s="10"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="B144" s="11"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="3">
+        <v>0.75209999999999999</v>
+      </c>
+      <c r="B145" s="11"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="3">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="6">
+        <v>0.75929999999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="8">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="6">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="6">
+        <v>0.76170000000000004</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="3">
+        <v>0.7631</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="6">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="3">
+        <v>0.77029999999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="6">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="3">
+        <v>0.77359999999999995</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="3">
+        <v>0.77759999999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="6">
+        <v>0.78149999999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="3">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="6">
+        <v>0.79520000000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="3">
+        <v>0.79530000000000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="8">
+        <v>0.80030000000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="3">
+        <v>0.83189999999999997</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="6">
+        <v>0.84450000000000003</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="6">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G107" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
+    <filterColumn colId="2">
       <filters>
-        <filter val="语音+视频"/>
-        <filter val="语音-视频-文本"/>
+        <filter val="IEMOCAP"/>
+        <filter val="IEMOCAP(VoxCeleb1)"/>
+        <filter val="IEMOCAP+Att-HACK"/>
+        <filter val="IEMOCAP+CMUMOSEI+DAIC-WOZ"/>
+        <filter val="IEMOCAP+CMUMOSI"/>
+        <filter val="IEMOCAP+CMU-MOSI"/>
+        <filter val="IEMOCAP+CREMA-D+MSP-Improv"/>
+        <filter val="IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast"/>
+        <filter val="IEMOCAP+DailyDialog+MELD+EmoryNLP"/>
+        <filter val="IEMOCAP+ESD"/>
+        <filter val="IEMOCAP+MELD"/>
+        <filter val="IEMOCAP+MSP-IMPROV"/>
+        <filter val="IEMOCAP+MSP-Improv+CREMA-D"/>
+        <filter val="IEMOCAP+MSP-Podcast"/>
+        <filter val="IEMOCAP+NNIME"/>
+        <filter val="IEMOCAP+RAVDESS"/>
+        <filter val="IEMOCAP+RAVDESS+Emo-DB"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G107">
       <sortCondition ref="A1:A107"/>
     </sortState>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A112:A166">
+    <sortCondition ref="A112:A166"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2024-02-26 12:31:52
</commit_message>
<xml_diff>
--- a/Research/情感语音/{2}_论文记录/情感识别论文统计.xlsx
+++ b/Research/情感语音/{2}_论文记录/情感识别论文统计.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\{3}_进修\{4}_笔记\Research\情感语音\{2}_论文记录\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4bf5f6a84bc81b7/同步/{4}_笔记/Research/情感语音/{2}_论文记录/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA5A4E-4A4B-42C3-B649-5534C16FB209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6BDA5A4E-4A4B-42C3-B649-5534C16FB209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDB6E16E-7DEE-46BE-B0C7-C8657325C151}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1104" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,401 +401,402 @@
     <t>Emotion Recognition by Fusing Time Synchronous and Time Asynchronous Representations</t>
   </si>
   <si>
+    <t>Disentanglement for Audio-Visual Emotion Recognition Using Multitask Setup</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks</t>
+  </si>
+  <si>
+    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions</t>
+  </si>
+  <si>
+    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Meta-Learning for Low-Resource Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition</t>
+  </si>
+  <si>
+    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks</t>
+  </si>
+  <si>
+    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection</t>
+  </si>
+  <si>
+    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions</t>
+  </si>
+  <si>
+    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
+  </si>
+  <si>
+    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
+  </si>
+  <si>
+    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
+  </si>
+  <si>
+    <t>Temporal Context in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
+  </si>
+  <si>
+    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
+  </si>
+  <si>
+    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
+  </si>
+  <si>
+    <t>Emotion Carrier Recognition from Personal Narratives</t>
+  </si>
+  <si>
+    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
+  </si>
+  <si>
+    <t>Emotional Prosody Control for Speech Generation</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
+  </si>
+  <si>
+    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
+  </si>
+  <si>
+    <t>Speaker Attentive Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
+  </si>
+  <si>
+    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
+  </si>
+  <si>
+    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
+  </si>
+  <si>
+    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
+  </si>
+  <si>
+    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
+  </si>
+  <si>
+    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
+  </si>
+  <si>
+    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMU-MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音+视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+ESD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmoDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.5±1.0%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wF1 78.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSI+CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音-视频-文本 </t>
+  </si>
+  <si>
+    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本 </t>
+  </si>
+  <si>
+    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wf1 65.85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MELD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emo-DB+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.6± 4.7% - 61.7±9.2%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMUMOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+NNIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-IMPROV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.613 ± 0.018%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+Att-HACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS+Emo-DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音 </t>
+  </si>
+  <si>
+    <t>67.2 ± 0.7%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95.90 ± 4.31%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本   </t>
+  </si>
+  <si>
+    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition with Multi-Task Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multimodal Emotion Recognition with Capsule Graph Convolutional Based Representation Fusion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>A Novel Attention-Based Gated Recurrent Unit and its Efficacy in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Disentanglement for Audio-Visual Emotion Recognition Using Multitask Setup</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks</t>
-  </si>
-  <si>
-    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions</t>
-  </si>
-  <si>
-    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Meta-Learning for Low-Resource Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition</t>
-  </si>
-  <si>
-    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks</t>
-  </si>
-  <si>
-    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection</t>
-  </si>
-  <si>
-    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions</t>
-  </si>
-  <si>
-    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
-  </si>
-  <si>
-    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
-  </si>
-  <si>
-    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
-  </si>
-  <si>
-    <t>Temporal Context in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
-  </si>
-  <si>
-    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
-  </si>
-  <si>
-    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
-  </si>
-  <si>
-    <t>Emotion Carrier Recognition from Personal Narratives</t>
-  </si>
-  <si>
-    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
-  </si>
-  <si>
-    <t>Emotional Prosody Control for Speech Generation</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
-  </si>
-  <si>
-    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
-  </si>
-  <si>
-    <t>Speaker Attentive Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
-  </si>
-  <si>
-    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
-  </si>
-  <si>
-    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
-  </si>
-  <si>
-    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
-  </si>
-  <si>
-    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
-  </si>
-  <si>
-    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
-  </si>
-  <si>
-    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMU-MOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音+视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+ESD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EmoDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>87.5±1.0%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wF1 78.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSI+CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音-视频-文本 </t>
-  </si>
-  <si>
-    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本 </t>
-  </si>
-  <si>
-    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wf1 65.85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emo-DB+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.6± 4.7% - 61.7±9.2%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMUMOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+NNIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-IMPROV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.613 ± 0.018%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+Att-HACK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS+Emo-DB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音 </t>
-  </si>
-  <si>
-    <t>67.2 ± 0.7%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95.90 ± 4.31%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本   </t>
-  </si>
-  <si>
-    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition with Multi-Task Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>√</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Multimodal Emotion Recognition with Capsule Graph Convolutional Based Representation Fusion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2253,26 +2254,26 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G136" sqref="G136"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="43.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.9140625" style="1"/>
+    <col min="6" max="6" width="16.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="43.75" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="21.109375" style="10" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="8.9140625" style="1"/>
+    <col min="10" max="10" width="21.08203125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="21.08203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.9140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2296,9 +2297,9 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>55</v>
@@ -2320,7 +2321,7 @@
         <v>100.21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -2346,9 +2347,9 @@
         <v>84.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -2370,7 +2371,7 @@
         <v>84.45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>83.19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -2415,12 +2416,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>54</v>
@@ -2436,19 +2437,19 @@
         <v>80.03</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1"/>
       <c r="L8" s="1">
         <v>79.53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -2469,15 +2470,15 @@
         <v>79.52</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G10" s="6">
         <v>0.65600000000000003</v>
@@ -2486,12 +2487,12 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="1"/>
       <c r="J11" s="10">
@@ -2501,7 +2502,7 @@
         <v>78.150000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -2524,9 +2525,9 @@
         <v>77.760000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>55</v>
@@ -2540,7 +2541,7 @@
         <v>77.36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>77.099999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -2585,12 +2586,12 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>54</v>
@@ -2606,15 +2607,15 @@
         <v>76.31</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>59</v>
@@ -2626,7 +2627,7 @@
         <v>76.17</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -2647,12 +2648,12 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="3"/>
@@ -2660,15 +2661,15 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G20" s="6">
         <v>0.6169</v>
@@ -2681,9 +2682,9 @@
         <v>75.930000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>55</v>
@@ -2692,10 +2693,10 @@
         <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G21" s="2">
         <v>73.22</v>
@@ -2707,7 +2708,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -2777,19 +2778,19 @@
         <v>73.22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G25" s="1"/>
       <c r="L25" s="1">
         <v>73.040000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2812,12 +2813,12 @@
         <v>72.83</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G27" s="1"/>
       <c r="J27" s="10">
@@ -2827,12 +2828,12 @@
         <v>72.48</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G28" s="1"/>
       <c r="J28" s="10">
@@ -2842,7 +2843,7 @@
         <v>70.819999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>83</v>
       </c>
@@ -2866,21 +2867,21 @@
         <v>70.540000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H30" s="3"/>
       <c r="J30" s="10">
@@ -2890,7 +2891,7 @@
         <v>70.459999999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
@@ -2914,9 +2915,9 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>55</v>
@@ -2927,15 +2928,15 @@
         <v>70.11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -2950,7 +2951,7 @@
         <v>69.760000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -2971,9 +2972,9 @@
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>14</v>
@@ -2992,29 +2993,29 @@
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L36" s="1">
         <v>68.17</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>55</v>
@@ -3036,9 +3037,9 @@
         <v>67.42</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
@@ -3056,9 +3057,9 @@
         <v>66.900000000000006</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>14</v>
@@ -3073,7 +3074,7 @@
         <v>66.900000000000006</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>86</v>
       </c>
@@ -3093,9 +3094,9 @@
         <v>65.599999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>56</v>
@@ -3117,12 +3118,12 @@
         <v>65.53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="3"/>
@@ -3133,15 +3134,15 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>53</v>
@@ -3157,7 +3158,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>88</v>
       </c>
@@ -3180,21 +3181,21 @@
         <v>61.69</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J45" s="10">
         <v>73.040000000000006</v>
@@ -3203,12 +3204,12 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G46" s="1"/>
       <c r="J46" s="10">
@@ -3218,15 +3219,15 @@
         <v>60.43</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -3241,12 +3242,12 @@
         <v>58.19</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="G48" s="1"/>
       <c r="J48" s="10">
@@ -3256,7 +3257,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>87</v>
       </c>
@@ -3280,9 +3281,9 @@
         <v>36.58</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>55</v>
@@ -3304,18 +3305,18 @@
         <v>0.77029999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -3326,15 +3327,15 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>53</v>
@@ -3345,9 +3346,9 @@
         <v>0.68189999999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>55</v>
@@ -3361,12 +3362,12 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -3377,15 +3378,15 @@
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>59</v>
@@ -3401,7 +3402,7 @@
         <v>0.62680000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -3425,9 +3426,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>55</v>
@@ -3436,7 +3437,7 @@
         <v>54</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G57" s="6">
         <v>0.84450000000000003</v>
@@ -3449,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -3473,15 +3474,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>59</v>
@@ -3497,12 +3498,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>54</v>
@@ -3518,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -3542,9 +3543,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>55</v>
@@ -3566,9 +3567,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>55</v>
@@ -3586,23 +3587,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H64" s="8"/>
       <c r="J64" s="11">
@@ -3612,15 +3613,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -3636,9 +3637,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>14</v>
@@ -3660,9 +3661,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>55</v>
@@ -3671,7 +3672,7 @@
         <v>54</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G67" s="8">
         <v>0.73040000000000005</v>
@@ -3684,9 +3685,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>14</v>
@@ -3706,12 +3707,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>54</v>
@@ -3728,15 +3729,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H70" s="8"/>
       <c r="J70" s="11"/>
@@ -3744,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
@@ -3765,9 +3766,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>14</v>
@@ -3783,7 +3784,7 @@
       </c>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>63</v>
       </c>
@@ -3804,9 +3805,9 @@
       <c r="H73" s="8"/>
       <c r="J73" s="11"/>
     </row>
-    <row r="74" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>55</v>
@@ -3820,7 +3821,7 @@
       <c r="H74" s="8"/>
       <c r="J74" s="11"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -3838,7 +3839,7 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
@@ -3856,7 +3857,7 @@
       </c>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>79</v>
       </c>
@@ -3876,9 +3877,9 @@
       </c>
       <c r="J77" s="11"/>
     </row>
-    <row r="78" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>56</v>
@@ -3887,22 +3888,22 @@
         <v>54</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J78" s="11"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
@@ -3912,49 +3913,49 @@
       </c>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G80" s="6">
         <v>0.77100000000000002</v>
       </c>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>14</v>
@@ -3970,7 +3971,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>62</v>
       </c>
@@ -3988,18 +3989,18 @@
       </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -4008,17 +4009,17 @@
       </c>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>74</v>
       </c>
@@ -4036,40 +4037,40 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G88" s="6">
         <v>0.76100000000000001</v>
       </c>
       <c r="H88" s="6"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -4087,9 +4088,9 @@
       </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>55</v>
@@ -4097,22 +4098,22 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>14</v>
@@ -4128,37 +4129,37 @@
       </c>
       <c r="H93" s="6"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G94" s="6">
         <v>0.70399999999999996</v>
       </c>
       <c r="H94" s="6"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G95" s="6">
         <v>0.61399999999999999</v>
       </c>
       <c r="H95" s="6"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>60</v>
       </c>
@@ -4179,50 +4180,50 @@
       </c>
       <c r="H96" s="6"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G97" s="6">
         <v>0.78149999999999997</v>
       </c>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="6"/>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>55</v>
@@ -4230,60 +4231,60 @@
       <c r="G100" s="1"/>
       <c r="H100" s="6"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G101" s="6">
         <v>0.75</v>
       </c>
       <c r="H101" s="6"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G102" s="6">
         <v>0.66900000000000004</v>
       </c>
       <c r="H102" s="6"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G103" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>55</v>
@@ -4299,12 +4300,12 @@
       </c>
       <c r="H104" s="6"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>54</v>
@@ -4314,9 +4315,9 @@
       </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>8</v>
@@ -4325,7 +4326,7 @@
         <v>32</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>16</v>
@@ -4335,18 +4336,18 @@
       </c>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -4355,330 +4356,330 @@
       </c>
       <c r="H107" s="6"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>0.36580000000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>0.57599999999999996</v>
       </c>
       <c r="B113" s="10"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>0.58189999999999997</v>
       </c>
       <c r="B114" s="10"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>0.60429999999999995</v>
       </c>
       <c r="B115" s="10"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>0.61399999999999999</v>
       </c>
       <c r="B116" s="10"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <v>0.6169</v>
       </c>
       <c r="B117" s="10"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>0.62680000000000002</v>
       </c>
       <c r="B118" s="10"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="8">
         <v>0.63100000000000001</v>
       </c>
       <c r="B119" s="10"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>0.63400000000000001</v>
       </c>
       <c r="B120" s="10"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <v>0.63400000000000001</v>
       </c>
       <c r="B121" s="10"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <v>0.65529999999999999</v>
       </c>
       <c r="B122" s="10"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <v>0.65600000000000003</v>
       </c>
       <c r="B123" s="10"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
         <v>0.65849999999999997</v>
       </c>
       <c r="B124" s="10"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>0.66900000000000004</v>
       </c>
       <c r="B125" s="10"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
         <v>0.66900000000000004</v>
       </c>
       <c r="B126" s="10"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="8">
         <v>0.67420000000000002</v>
       </c>
       <c r="B127" s="10"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
         <v>0.67900000000000005</v>
       </c>
       <c r="B128" s="10"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="8">
         <v>0.68169999999999997</v>
       </c>
       <c r="B129" s="10"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>0.68189999999999995</v>
       </c>
       <c r="B130" s="10"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>0.68210000000000004</v>
       </c>
       <c r="B131" s="10"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="8">
         <v>0.68899999999999995</v>
       </c>
       <c r="B132" s="10"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>0.6976</v>
       </c>
       <c r="B133" s="10"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="8">
         <v>0.70109999999999995</v>
       </c>
       <c r="B134" s="10"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
         <v>0.70399999999999996</v>
       </c>
       <c r="B135" s="10"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>0.7046</v>
       </c>
       <c r="B136" s="10"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>0.70540000000000003</v>
       </c>
       <c r="B137" s="10"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
         <v>0.70820000000000005</v>
       </c>
       <c r="B138" s="10"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>0.7248</v>
       </c>
       <c r="B139" s="10"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
         <v>0.72829999999999995</v>
       </c>
       <c r="B140" s="10"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>0.73040000000000005</v>
       </c>
       <c r="B141" s="10"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>0.73219999999999996</v>
       </c>
       <c r="B142" s="10"/>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
         <v>0.73499999999999999</v>
       </c>
       <c r="B143" s="10"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
         <v>0.75</v>
       </c>
       <c r="B144" s="11"/>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>0.75209999999999999</v>
       </c>
       <c r="B145" s="11"/>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
         <v>0.75929999999999997</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
         <v>0.76170000000000004</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>0.7631</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>0.77029999999999998</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>0.77359999999999995</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>0.77759999999999996</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
         <v>0.78149999999999997</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
         <v>0.79520000000000002</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>0.79530000000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="8">
         <v>0.80030000000000001</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>0.81</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>0.83189999999999997</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
         <v>0.84450000000000003</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
         <v>0.84499999999999997</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G107" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="ICASSP2021"/>
+        <filter val="ICASSP2022"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="IEMOCAP"/>
         <filter val="IEMOCAP(VoxCeleb1)"/>
-        <filter val="IEMOCAP+Att-HACK"/>
-        <filter val="IEMOCAP+CMUMOSEI+DAIC-WOZ"/>
-        <filter val="IEMOCAP+CMUMOSI"/>
-        <filter val="IEMOCAP+CMU-MOSI"/>
-        <filter val="IEMOCAP+CREMA-D+MSP-Improv"/>
-        <filter val="IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast"/>
-        <filter val="IEMOCAP+DailyDialog+MELD+EmoryNLP"/>
-        <filter val="IEMOCAP+ESD"/>
         <filter val="IEMOCAP+MELD"/>
-        <filter val="IEMOCAP+MSP-IMPROV"/>
         <filter val="IEMOCAP+MSP-Improv+CREMA-D"/>
         <filter val="IEMOCAP+MSP-Podcast"/>
-        <filter val="IEMOCAP+NNIME"/>
-        <filter val="IEMOCAP+RAVDESS"/>
-        <filter val="IEMOCAP+RAVDESS+Emo-DB"/>
+        <filter val="IEMOCAP+RAVDESS+EMO-DB"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="语音"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G107">

</xml_diff>